<commit_message>
Fehler in Test-Excel verbaut
</commit_message>
<xml_diff>
--- a/src/test/resources/Fragenkatalog.xlsx
+++ b/src/test/resources/Fragenkatalog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7995" tabRatio="930" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15315" windowHeight="7995" tabRatio="930" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,12 @@
     <sheet name="GS54" sheetId="26" r:id="rId25"/>
     <sheet name="Jugend" sheetId="29" r:id="rId26"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3152" uniqueCount="2555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3146" uniqueCount="2555">
   <si>
     <t>Frage</t>
   </si>
@@ -12197,7 +12197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -18641,10 +18641,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -18654,368 +18654,369 @@
     <col min="6" max="6" width="31.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="29.25">
+    <row r="1" spans="1:6" ht="29.25">
+      <c r="A1" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" s="24">
+        <v>24</v>
+      </c>
+      <c r="C1" s="24">
+        <v>26</v>
+      </c>
+      <c r="D1" s="24">
+        <v>27</v>
+      </c>
+      <c r="E1" s="24">
+        <v>30</v>
+      </c>
+      <c r="F1" s="24">
+        <f>E1</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="24">
-        <v>24</v>
-      </c>
-      <c r="C2" s="24">
-        <v>26</v>
-      </c>
-      <c r="D2" s="24">
-        <v>27</v>
-      </c>
-      <c r="E2" s="24">
-        <v>30</v>
-      </c>
-      <c r="F2" s="24">
-        <f>E2</f>
-        <v>30</v>
+        <v>131</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" s="24" t="str">
+        <f>C2</f>
+        <v>Anzug &amp; Krawatte</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="24" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F3" s="24" t="str">
-        <f>C3</f>
-        <v>Anzug &amp; Krawatte</v>
+        <f>D3</f>
+        <v>980,- EUR</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="24" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>137</v>
       </c>
       <c r="C4" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="24" t="s">
-        <v>140</v>
-      </c>
       <c r="E4" s="24" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F4" s="24" t="str">
-        <f>D4</f>
-        <v>980,- EUR</v>
+        <f>E4</f>
+        <v>930,- EUR</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="24" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>137</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F5" s="24" t="str">
-        <f>E5</f>
-        <v>930,- EUR</v>
+        <f>D5</f>
+        <v>1040,- EUR</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="24" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="F6" s="24" t="str">
-        <f>D6</f>
-        <v>1040,- EUR</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <f>C6</f>
+        <v>2,5 Jahre</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29.25">
       <c r="A7" s="24" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="F7" s="24" t="str">
         <f>C7</f>
-        <v>2,5 Jahre</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="29.25">
+        <v xml:space="preserve">1 Jahr vorher </v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="F8" s="24" t="str">
-        <f>C8</f>
-        <v xml:space="preserve">1 Jahr vorher </v>
+        <f>B8</f>
+        <v>Übers Internet</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="24" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="F9" s="24" t="str">
-        <f>B9</f>
-        <v>Übers Internet</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <f>C9</f>
+        <v xml:space="preserve">August </v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29.25">
       <c r="A10" s="24" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
       <c r="F10" s="24" t="str">
         <f>C10</f>
-        <v xml:space="preserve">August </v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="29.25">
+        <v>Verschiedene Geschäftsstellen</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="24" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="F11" s="24" t="str">
         <f>C11</f>
-        <v>Verschiedene Geschäftsstellen</v>
+        <v>Goch</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="24" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F12" s="24" t="str">
-        <f>C12</f>
-        <v>Goch</v>
+        <f>B12</f>
+        <v>Prüfungs-TV</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F13" s="24" t="str">
-        <f>B13</f>
-        <v>Prüfungs-TV</v>
+        <f>D13</f>
+        <v xml:space="preserve">Studium </v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="24" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F14" s="24" t="str">
-        <f>D14</f>
-        <v xml:space="preserve">Studium </v>
+        <f>E14</f>
+        <v>Überbetrieblicher Unterricht</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="24" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="F15" s="24" t="str">
-        <f>E15</f>
-        <v>Überbetrieblicher Unterricht</v>
+        <f>C15</f>
+        <v>2x in 1 Woche</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="24" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F16" s="24" t="str">
         <f>C16</f>
-        <v>2x in 1 Woche</v>
+        <v>wöchentlicher Unterricht</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="24" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F17" s="24" t="str">
-        <f>C17</f>
-        <v>wöchentlicher Unterricht</v>
+        <f>D17</f>
+        <v xml:space="preserve">1x in 1 Woche </v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="24" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C18" s="24" t="s">
         <v>190</v>
@@ -19027,481 +19028,460 @@
         <v>192</v>
       </c>
       <c r="F18" s="24" t="str">
-        <f>D18</f>
-        <v xml:space="preserve">1x in 1 Woche </v>
+        <f>B18</f>
+        <v>3x in 2 Wochen</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="24" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="F19" s="24" t="str">
         <f>B19</f>
-        <v>3x in 2 Wochen</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>Abschlussprüfung</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="29.25">
       <c r="A20" s="24" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F20" s="24" t="str">
-        <f>B20</f>
-        <v>Abschlussprüfung</v>
+        <f>E20</f>
+        <v>vermögenswirksame Leistungen</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="29.25">
       <c r="A21" s="24" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="F21" s="24" t="str">
-        <f>E21</f>
-        <v>vermögenswirksame Leistungen</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="29.25">
+        <f>D21</f>
+        <v>Postverteilung</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="24" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="F22" s="24" t="str">
-        <f>D22</f>
-        <v>Postverteilung</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <f>B22</f>
+        <v>Abzug der Steuern</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="29.25">
       <c r="A23" s="24" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="F23" s="24" t="str">
-        <f>B23</f>
-        <v>Abzug der Steuern</v>
+        <f>E23</f>
+        <v>Facebook</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29.25">
       <c r="A24" s="24" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>225</v>
+        <v>159</v>
       </c>
       <c r="F24" s="24" t="str">
-        <f>E24</f>
-        <v>Facebook</v>
+        <f>C24</f>
+        <v>Paddeln</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="29.25">
       <c r="A25" s="24" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>159</v>
+        <v>239</v>
       </c>
       <c r="F25" s="24" t="str">
-        <f>C25</f>
-        <v>Paddeln</v>
+        <f>B25</f>
+        <v>Vorstellungstreffen</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="29.25">
       <c r="A26" s="24" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="F26" s="24" t="str">
-        <f>B26</f>
-        <v>Vorstellungstreffen</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="29.25">
-      <c r="A27" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>228</v>
-      </c>
-      <c r="D27" s="24" t="s">
-        <v>229</v>
-      </c>
-      <c r="E27" s="24" t="s">
-        <v>231</v>
-      </c>
-      <c r="F27" s="24" t="str">
-        <f>C27</f>
+        <f>C26</f>
         <v>Kennenlernprojekt in Forsbach</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="39" t="s">
+        <v>2554</v>
+      </c>
+      <c r="B27" s="39" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>2485</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>2486</v>
+      </c>
+      <c r="E27" s="39" t="s">
+        <v>2487</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>2484</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="39" t="s">
-        <v>2554</v>
+        <v>2488</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>2484</v>
+        <v>2489</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>2485</v>
+        <v>2490</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>2486</v>
+        <v>212</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>2487</v>
+        <v>2491</v>
       </c>
       <c r="F28" s="39" t="s">
-        <v>2484</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>2491</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="29.25">
       <c r="A29" s="39" t="s">
-        <v>2488</v>
+        <v>2553</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>2489</v>
+        <v>2492</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>2490</v>
+        <v>2493</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>212</v>
+        <v>2494</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>2491</v>
+        <v>2495</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>2491</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="29.25">
       <c r="A30" s="39" t="s">
-        <v>2553</v>
+        <v>2496</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>2492</v>
+        <v>2497</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>2493</v>
+        <v>2498</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>2494</v>
+        <v>2499</v>
       </c>
       <c r="E30" s="39" t="s">
-        <v>2495</v>
+        <v>2500</v>
       </c>
       <c r="F30" s="39" t="s">
-        <v>2492</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="29.25">
       <c r="A31" s="39" t="s">
-        <v>2496</v>
+        <v>2552</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>2497</v>
+        <v>2501</v>
       </c>
       <c r="C31" s="39" t="s">
-        <v>2498</v>
+        <v>2502</v>
       </c>
       <c r="D31" s="39" t="s">
-        <v>2499</v>
+        <v>2503</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>2500</v>
+        <v>2504</v>
       </c>
       <c r="F31" s="39" t="s">
-        <v>2499</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="29.25">
+        <v>2501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="39" t="s">
-        <v>2552</v>
+        <v>2505</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>2501</v>
+        <v>2506</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>2502</v>
+        <v>2507</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>2503</v>
+        <v>2508</v>
       </c>
       <c r="E32" s="39" t="s">
-        <v>2504</v>
+        <v>2509</v>
       </c>
       <c r="F32" s="39" t="s">
-        <v>2501</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="29.25">
       <c r="A33" s="39" t="s">
-        <v>2505</v>
+        <v>2510</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>2506</v>
+        <v>2511</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>2507</v>
+        <v>2512</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>2508</v>
+        <v>2513</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>2509</v>
+        <v>2514</v>
       </c>
       <c r="F33" s="39" t="s">
-        <v>2507</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="29.25">
       <c r="A34" s="39" t="s">
-        <v>2510</v>
+        <v>2515</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>2511</v>
+        <v>2516</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>2512</v>
+        <v>2517</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>2513</v>
+        <v>2518</v>
       </c>
       <c r="E34" s="39" t="s">
-        <v>2514</v>
+        <v>2519</v>
       </c>
       <c r="F34" s="39" t="s">
-        <v>2513</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="29.25">
       <c r="A35" s="39" t="s">
-        <v>2515</v>
+        <v>2520</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>2516</v>
+        <v>2521</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>2517</v>
+        <v>2522</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>2518</v>
+        <v>175</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>2519</v>
+        <v>2523</v>
       </c>
       <c r="F35" s="39" t="s">
-        <v>2516</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="29.25">
       <c r="A36" s="39" t="s">
-        <v>2520</v>
+        <v>2524</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>2521</v>
+        <v>2525</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>2522</v>
+        <v>2548</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>175</v>
+        <v>2526</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>2523</v>
-      </c>
-      <c r="F36" s="39" t="s">
-        <v>2522</v>
+        <v>2527</v>
+      </c>
+      <c r="F36" s="39" t="str">
+        <f>C36</f>
+        <v>5 Monate</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="29.25">
       <c r="A37" s="39" t="s">
-        <v>2524</v>
+        <v>2530</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>2525</v>
+        <v>2531</v>
       </c>
       <c r="C37" s="39" t="s">
-        <v>2548</v>
+        <v>2532</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>2526</v>
+        <v>2549</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>2527</v>
+        <v>2533</v>
       </c>
       <c r="F37" s="39" t="str">
-        <f>C37</f>
-        <v>5 Monate</v>
+        <f>D37</f>
+        <v>Accessmentcenter</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="29.25">
       <c r="A38" s="39" t="s">
-        <v>2530</v>
+        <v>2550</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>2531</v>
+        <v>2534</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>2532</v>
+        <v>2535</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>2549</v>
+        <v>2536</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>2533</v>
+        <v>2537</v>
       </c>
       <c r="F38" s="39" t="str">
-        <f>D38</f>
-        <v>Accessmentcenter</v>
+        <f>B38</f>
+        <v>Fachwissen</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="29.25">
       <c r="A39" s="39" t="s">
-        <v>2550</v>
+        <v>2538</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>2534</v>
+        <v>2539</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>2535</v>
+        <v>2540</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>2536</v>
+        <v>2541</v>
       </c>
       <c r="E39" s="39" t="s">
-        <v>2537</v>
+        <v>2542</v>
       </c>
       <c r="F39" s="39" t="str">
-        <f>B39</f>
-        <v>Fachwissen</v>
+        <f>D39</f>
+        <v>Nur Topverdiener können Kunden werden</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="29.25">
       <c r="A40" s="39" t="s">
-        <v>2538</v>
+        <v>2543</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>2539</v>
+        <v>2544</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>2540</v>
+        <v>2545</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>2541</v>
+        <v>2546</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>2542</v>
+        <v>2547</v>
       </c>
       <c r="F40" s="39" t="str">
-        <f>D40</f>
-        <v>Nur Topverdiener können Kunden werden</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="29.25">
-      <c r="A41" s="39" t="s">
-        <v>2543</v>
-      </c>
-      <c r="B41" s="39" t="s">
-        <v>2544</v>
-      </c>
-      <c r="C41" s="39" t="s">
-        <v>2545</v>
-      </c>
-      <c r="D41" s="39" t="s">
-        <v>2546</v>
-      </c>
-      <c r="E41" s="39" t="s">
-        <v>2547</v>
-      </c>
-      <c r="F41" s="39" t="str">
-        <f>C41</f>
+        <f>C40</f>
         <v>Brauchtumstage</v>
       </c>
     </row>

</xml_diff>